<commit_message>
update P50 class list
</commit_message>
<xml_diff>
--- a/studentList_P50.xlsx
+++ b/studentList_P50.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/int/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D77DEA0-B7B4-D549-8928-D9E1CC463593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C5EC85-337A-B24B-AA71-BD26B9B3995B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44020" yWindow="5380" windowWidth="22140" windowHeight="21380" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
   </bookViews>
@@ -34,68 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Students</t>
   </si>
   <si>
-    <t>BOROWSKY, KATHERINE JANE</t>
-  </si>
-  <si>
-    <t>DROBNY, TEDDY</t>
-  </si>
-  <si>
-    <t>EINSTEIN, MAXIMILLIAN H.</t>
-  </si>
-  <si>
-    <t>KUNGVAL, PHORNTHAP</t>
-  </si>
-  <si>
-    <t>LI, FUTONG</t>
-  </si>
-  <si>
-    <t>LINDLEY, JADEN JAMES</t>
-  </si>
-  <si>
-    <t>MA, HARRISON QIAN JUNLI</t>
-  </si>
-  <si>
-    <t>NGUYEN, CHRISTINE VY</t>
-  </si>
-  <si>
-    <t>RAPPARPORT, CATHERINE SIMONE</t>
-  </si>
-  <si>
-    <t>RIOS, IZAAC ANTHONY</t>
-  </si>
-  <si>
-    <t>WU, YUDONG</t>
-  </si>
-  <si>
-    <t>YAN, RUOQI</t>
-  </si>
-  <si>
-    <t>ZHANG, ZHANZHI</t>
-  </si>
-  <si>
-    <t>ZHAO, SHAOCHONG</t>
-  </si>
-  <si>
-    <t>Katherine</t>
-  </si>
-  <si>
     <t>Teddy</t>
   </si>
   <si>
-    <t>Maximillian</t>
-  </si>
-  <si>
-    <t>Phornthap</t>
-  </si>
-  <si>
-    <t>Futong</t>
-  </si>
-  <si>
     <t>Jaden</t>
   </si>
   <si>
@@ -111,23 +57,35 @@
     <t>Izaac</t>
   </si>
   <si>
-    <t>Yudong</t>
-  </si>
-  <si>
-    <t>Ruoqi</t>
-  </si>
-  <si>
-    <t>Zhanshi</t>
-  </si>
-  <si>
-    <t>Shaochong</t>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Wallace</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Katie</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Zhanzhiz</t>
+  </si>
+  <si>
+    <t>Ryan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,6 +106,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,10 +135,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -490,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126A2D9E-F695-4645-8524-97D12A4669B8}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,12 +469,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -517,12 +480,10 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -530,12 +491,10 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="2"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -543,12 +502,10 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -556,12 +513,10 @@
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -569,12 +524,10 @@
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -582,12 +535,10 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -595,12 +546,10 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -608,12 +557,10 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -621,12 +568,10 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -634,12 +579,10 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -647,12 +590,10 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -660,12 +601,10 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -673,19 +612,23 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add student to P50
</commit_message>
<xml_diff>
--- a/studentList_P50.xlsx
+++ b/studentList_P50.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/int/makeSmallGroups/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FF40B5-D437-2B4B-86AE-098D07FA27C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32D86ED-F0EE-3A46-806F-DAF048D04678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45380" yWindow="3580" windowWidth="22140" windowHeight="21380" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
+    <workbookView xWindow="15140" yWindow="2320" windowWidth="13000" windowHeight="11340" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>Students</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Daniel</t>
+  </si>
+  <si>
+    <t>Shaochong</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K38" sqref="D2:K38"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,6 +694,11 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="4:5" x14ac:dyDescent="0.2">

</xml_diff>